<commit_message>
update log as per class
</commit_message>
<xml_diff>
--- a/automation-exercise-cucumberuntitled/test-output/ExcelReport/ExtentExcel.xlsx
+++ b/automation-exercise-cucumberuntitled/test-output/ExcelReport/ExtentExcel.xlsx
@@ -189,28 +189,28 @@
     <t>device</t>
   </si>
   <si>
-    <t>Jan 01, 2024 2:58:59 PM</t>
+    <t>Jan 01, 2024 5:11:44 PM</t>
   </si>
   <si>
-    <t>Jan 01, 2024 2:58:36 PM</t>
+    <t>Jan 01, 2024 5:09:34 PM</t>
   </si>
   <si>
-    <t>Jan 01, 2024 2:58:56 PM</t>
+    <t>Jan 01, 2024 5:11:38 PM</t>
   </si>
   <si>
-    <t>20.423 s</t>
+    <t>2 m 4.207 s</t>
   </si>
   <si>
     <t>100%</t>
   </si>
   <si>
-    <t>User should download Invoice after purchase order.</t>
+    <t>User should verify address details in checkout page</t>
   </si>
   <si>
-    <t>19.533 s</t>
+    <t>2 m 3.209 s</t>
   </si>
   <si>
-    <t>Product page and Product Details</t>
+    <t>Register Feature</t>
   </si>
   <si>
     <t>@author_JignashThummar</t>
@@ -219,10 +219,10 @@
     <t>@regression</t>
   </si>
   <si>
-    <t>@testing</t>
+    <t>@register</t>
   </si>
   <si>
-    <t>19.540 s</t>
+    <t>2 m 3.215 s</t>
   </si>
 </sst>
 </file>
@@ -2188,7 +2188,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>User should download Invoice after purchase order.</c:v>
+                  <c:v>User should verify address details in checkout page</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2199,7 +2199,7 @@
               <c:numCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2.0</c:v>
+                  <c:v>18.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2260,7 +2260,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>User should download Invoice after purchase order.</c:v>
+                  <c:v>User should verify address details in checkout page</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2327,7 +2327,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>User should download Invoice after purchase order.</c:v>
+                  <c:v>User should verify address details in checkout page</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2740,7 +2740,7 @@
                   <c:v>@regression</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>@testing</c:v>
+                  <c:v>@register</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2825,7 +2825,7 @@
                   <c:v>@regression</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>@testing</c:v>
+                  <c:v>@register</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2899,7 +2899,7 @@
                   <c:v>@regression</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>@testing</c:v>
+                  <c:v>@register</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3115,7 +3115,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Product page and Product Details</c:v>
+                  <c:v>Register Feature</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3187,7 +3187,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Product page and Product Details</c:v>
+                  <c:v>Register Feature</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3254,7 +3254,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Product page and Product Details</c:v>
+                  <c:v>Register Feature</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6197,7 +6197,7 @@
     <col min="7" max="7" customWidth="true" width="20.85546875"/>
   </cols>
   <sheetData/>
-  <sheetProtection sheet="true" password="CF63" scenarios="true" objects="true"/>
+  <sheetProtection sheet="true" password="D4F5" scenarios="true" objects="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -6287,10 +6287,10 @@
         <v>29</v>
       </c>
       <c r="G22" s="58" t="n">
-        <v>2.0</v>
+        <v>18.0</v>
       </c>
       <c r="H22" s="59" t="n">
-        <v>2.0</v>
+        <v>18.0</v>
       </c>
       <c r="I22" s="60"/>
       <c r="J22" s="61"/>
@@ -6593,10 +6593,10 @@
         <v>54</v>
       </c>
       <c r="J22" s="112" t="n">
-        <v>2.0</v>
+        <v>18.0</v>
       </c>
       <c r="K22" s="113" t="n">
-        <v>2.0</v>
+        <v>18.0</v>
       </c>
       <c r="L22" s="114"/>
       <c r="M22" s="115"/>
@@ -6675,7 +6675,7 @@
         <v>12</v>
       </c>
       <c r="H2" t="n" s="0">
-        <v>2.0</v>
+        <v>18.0</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -6744,7 +6744,7 @@
       </c>
       <c r="H5" t="n" s="0">
         <f>SUM(H2:H4)</f>
-        <v>2.0</v>
+        <v>18.0</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>